<commit_message>
Add Praveen Aiya solar project data and analysis
Added new directory 'Praveen Aiya' with data files, analysis notebook, and visualizations for the EE256 Solar Project. Updated and reorganized assignment and project description files, and replaced Task 4 document with a new version. Also updated PV.xlsx and Assignment 2025[1].docx with latest data.
</commit_message>
<xml_diff>
--- a/Solar Plant Design/PV.xlsx
+++ b/Solar Plant Design/PV.xlsx
@@ -5,30 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U S E R\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Semester 4\EE256 - Energy &amp; Power\Interactive NoteBoook\Power-and-Energy-Systems\Solar Plant Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF5A0A8-48A8-4962-B534-BC31993762C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAF21BE-B83A-406E-87E9-09D2B74A4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Energy Demand" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -125,17 +112,17 @@
     <t>Total per week</t>
   </si>
   <si>
-    <t>Total Annually (52 weeks)</t>
-  </si>
-  <si>
     <t>Total  per day for 90 rooms</t>
+  </si>
+  <si>
+    <t>Total Annually (52 weeks)/KWh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,16 +135,30 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -165,13 +166,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,570 +565,642 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="83" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.06</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
         <v>2.4E-2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>0.16600000000000001</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="3">
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>0.45</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
         <v>0.06</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="3">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="16"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
         <v>0.14399999999999999</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="G11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2">
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>0.9</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="G12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
         <v>0.06</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="3">
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>0.16600000000000001</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="3">
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="7"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
         <v>0.3</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="G17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7">
         <v>0.06</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="7">
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="18">
         <f>SUM(D2:D18)*90</f>
         <v>229.07699999999997</v>
       </c>
-      <c r="H22">
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="18">
         <f>SUM(H2:H18)*90</f>
         <v>202.13999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="14">
         <v>6</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="D30" s="11">
+        <v>10</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+      <c r="H30" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="13">
         <v>0.6</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G31" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31">
+      <c r="G31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="16">
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="11">
         <v>6</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="G33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="1">
-        <v>10</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="D34" s="11">
+        <v>10</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="H34" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14">
         <v>6</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1">
+      <c r="G36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="11">
         <v>8</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="12">
         <v>3.6</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G38" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38">
+      <c r="G38" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="5">
         <v>3.6</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="11">
         <v>6</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="1">
+      <c r="G40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="13">
         <v>1.44</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41">
+      <c r="G41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="16">
         <v>1.44</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -961,7 +1208,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -969,37 +1216,48 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D45">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="18">
         <f>SUM(D22:D41)</f>
         <v>286.71699999999998</v>
       </c>
-      <c r="H45">
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="18">
         <f>SUM(H22:H41)</f>
         <v>259.77999999999992</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D46">
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="13">
         <f>D45*7</f>
         <v>2007.0189999999998</v>
       </c>
-      <c r="H46">
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="13">
         <f>H45*2</f>
         <v>519.55999999999983</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:8" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="24">
         <f>(D46+H46)*52</f>
         <v>131382.10799999998</v>
       </c>

</xml_diff>